<commit_message>
commiting after several inconsistent test runs.
</commit_message>
<xml_diff>
--- a/result/testResult.xlsx
+++ b/result/testResult.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="15045" windowHeight="6405"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="11715" windowHeight="3855"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="data" r:id="rId7" sheetId="4"/>
   </sheets>
   <calcPr calcId="124519"/>
   <oleSize ref="A1:G10"/>
@@ -17,18 +18,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>Apple iPhone X (Silver, 64 GB)</t>
-  </si>
-  <si>
-    <t>[[ChromeDriver: chrome on XP (76f6c00741495541763e2fac4bf6cee6)] -&gt; xpath: //div[@class='_1vC4OE _2rQ-NK']]</t>
   </si>
 </sst>
 </file>
@@ -363,25 +355,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="42.140625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="39.85546875" collapsed="true"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -408,4 +389,22 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Still inconsistancy in the tests. modified the generic methods.
</commit_message>
<xml_diff>
--- a/result/testResult.xlsx
+++ b/result/testResult.xlsx
@@ -4,23 +4,140 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="11715" windowHeight="3855"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="14385" windowHeight="3765" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="data" r:id="rId7" sheetId="4"/>
+    <sheet name="data" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:G10"/>
+  <oleSize ref="A1:B1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1205" uniqueCount="40">
   <si>
     <t>Apple iPhone X (Silver, 64 GB)</t>
+  </si>
+  <si>
+    <t>Apple iPhone XR (Yellow, 256 GB)</t>
+  </si>
+  <si>
+    <t>₹74,900</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Apple iPhone X (Space Gray, 64 GB)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 6s (Rose Gold, 32 GB)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 6s (Silver, 32 GB)</t>
+  </si>
+  <si>
+    <t>Apple iPhone XR (Black, 64 GB)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 6s (Space Grey, 32 GB)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 6s Plus (Silver, 32 GB)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 6s Plus (Space Grey, 32 GB)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 6s (Gold, 32 GB)</t>
+  </si>
+  <si>
+    <t>Apple iPhone XR (Black, 128 GB)</t>
+  </si>
+  <si>
+    <t>Apple iPhone XR ((PRODUCT)RED, 64 GB)</t>
+  </si>
+  <si>
+    <t>Apple iPhone XR (White, 64 GB)</t>
+  </si>
+  <si>
+    <t>Apple iPhone XR (White, 128 GB)</t>
+  </si>
+  <si>
+    <t>Apple iPhone XR (Blue, 64 GB)</t>
+  </si>
+  <si>
+    <t>Apple iPhone XR (Coral, 128 GB)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 6s Plus (Gold, 32 GB)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 7 (Silver, 32 GB)</t>
+  </si>
+  <si>
+    <t>Apple iPhone XR (Blue, 128 GB)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 7 (Rose Gold, 128 GB)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 6s Plus (Silver, 16 GB)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 8 (PRODUCT)RED (Red, 64 GB)</t>
+  </si>
+  <si>
+    <t>Apple iPhone XR (Coral, 64 GB)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 8 (Gold, 64 GB)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 8 Plus (Gold, 64 GB)</t>
+  </si>
+  <si>
+    <t>₹69,999</t>
+  </si>
+  <si>
+    <t>₹29,799</t>
+  </si>
+  <si>
+    <t>₹59,900</t>
+  </si>
+  <si>
+    <t>₹29,590</t>
+  </si>
+  <si>
+    <t>₹34,900</t>
+  </si>
+  <si>
+    <t>₹64,900</t>
+  </si>
+  <si>
+    <t>₹39,990</t>
+  </si>
+  <si>
+    <t>₹39,900</t>
+  </si>
+  <si>
+    <t>₹52,990</t>
+  </si>
+  <si>
+    <t>₹54,999</t>
+  </si>
+  <si>
+    <t>₹59,490</t>
+  </si>
+  <si>
+    <t>₹58,999</t>
   </si>
 </sst>
 </file>
@@ -353,16 +470,217 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="42.140625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="39.85546875" collapsed="true"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -392,19 +710,33 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="44.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="26.28515625" collapsed="true"/>
+  </cols>
   <sheetData>
-    <row r="2">
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final Commit. Test Script executing as expected.
</commit_message>
<xml_diff>
--- a/result/testResult.xlsx
+++ b/result/testResult.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80153" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80753" uniqueCount="45">
   <si>
     <t>Apple iPhone X (Silver, 64 GB)</t>
   </si>
@@ -537,10 +537,10 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -553,26 +553,26 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -585,10 +585,10 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -601,18 +601,18 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -625,66 +625,66 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:2">

</xml_diff>